<commit_message>
Removed elec config, added sample freq in its place.
</commit_message>
<xml_diff>
--- a/my_batch.xlsx
+++ b/my_batch.xlsx
@@ -28,13 +28,13 @@
     <t xml:space="preserve">file_name</t>
   </si>
   <si>
-    <t xml:space="preserve">elec_config</t>
-  </si>
-  <si>
     <t xml:space="preserve">min_pk_height</t>
   </si>
   <si>
     <t xml:space="preserve">min_pk_dist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_frequency</t>
   </si>
   <si>
     <t xml:space="preserve">toggle_trunc</t>
@@ -122,6 +122,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -143,11 +144,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,16 +236,16 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.18"/>
@@ -289,19 +292,21 @@
       <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>120</v>
+      <c r="C2" s="2" t="n">
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -315,19 +320,21 @@
       <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="n">
-        <v>120</v>
+      <c r="C3" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J3" s="0" t="s">
@@ -341,19 +348,21 @@
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>120</v>
+      <c r="C4" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -364,19 +373,21 @@
       <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>120</v>
+      <c r="C5" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -387,19 +398,21 @@
       <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>120</v>
+      <c r="C6" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J6" s="0" t="s">
@@ -413,16 +426,17 @@
       <c r="B7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="n">
-        <v>120</v>
+      <c r="C7" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F7" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -431,7 +445,8 @@
       <c r="H7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I7" s="3" t="b">
+      <c r="I7" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -442,16 +457,17 @@
       <c r="B8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="n">
-        <v>120</v>
+      <c r="C8" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F8" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -460,7 +476,8 @@
       <c r="H8" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="b">
+      <c r="I8" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -471,19 +488,21 @@
       <c r="B9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>120</v>
+      <c r="C9" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J9" s="0" t="s">
@@ -497,19 +516,21 @@
       <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="n">
-        <v>120</v>
+      <c r="C10" s="2" t="n">
+        <v>150</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J10" s="0" t="s">
@@ -523,16 +544,17 @@
       <c r="B11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="n">
-        <v>120</v>
+      <c r="C11" s="2" t="n">
+        <v>125</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>125</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F11" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -541,7 +563,8 @@
       <c r="H11" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I11" s="3" t="b">
+      <c r="I11" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -552,19 +575,21 @@
       <c r="B12" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="n">
-        <v>120</v>
+      <c r="C12" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -575,19 +600,21 @@
       <c r="B13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="n">
-        <v>120</v>
+      <c r="C13" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -598,19 +625,21 @@
       <c r="B14" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="n">
-        <v>120</v>
+      <c r="C14" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3" t="b">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J14" s="0" t="s">
@@ -619,11 +648,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updated to fix issue (xlsx), attempt to normalize (others)
</commit_message>
<xml_diff>
--- a/my_batch.xlsx
+++ b/my_batch.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t xml:space="preserve">file_dir</t>
   </si>
@@ -107,6 +107,150 @@
   </si>
   <si>
     <t xml:space="preserve">B8, B7, A7, A6, C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/6-11-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip_9-6-11-18_Temp-37_1C.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E8, A9, K4, J8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/6-13-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip_9-6-13-18_Temp-37_1C.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/6-15-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip_9-6-15-18_Temp-37_1C.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7, A6, B6, A5, F4, F2, G3, J8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/Misc Data/Franky 2014 Sample 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day1 oct 24.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day1 oct 24 430pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day2 oct 25 1230pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B9, C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day3 oct 26  2pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day4 oct 27  1050am.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day4 oct 27  8pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day5 oct 28  5pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3, B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day6 oct 29 1100am.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day6 oct 29 430pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day7 oct 30 1100am.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3, B4, M6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day7 oct 30 5pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day8 oct 31 1045am.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day8 oct 31 4pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3, F3, H1, M6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample 2 Day9 Nov 1 2pm.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E12, B3, J12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/Kelsey Ion Blocker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-29-2016 No9_nifedipine_1_1nM.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F12, F11, D11, C10, E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-29-2016 No9_nifedipine_2_3nM.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F11, H9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-29-2016 No9_nifedipine_3_5nM.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/Kelsey Ion Blocker/Test&amp;Failed Data/09-15-2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No12_Pre_media only_Post0002.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3, G5, G2, G3, G4, H4, H5, K10, K11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No12_Post_CBX_50uM_Run2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/media/csdunham/0E24340D2433F675/Gimzewski Lab/Stem Cells/Data Sets/HES CM D33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D3 (9pm).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D3.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D4 (9am +12h w DAPT 2uM).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D5 (DAPT 2uM).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D6 (DAPT 2uM).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D7 (DAPT 2uM).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3100_Matrigel D8 (DAPT 2uM).txt</t>
   </si>
 </sst>
 </file>
@@ -233,16 +377,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="105.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
@@ -647,12 +791,786 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>